<commit_message>
feat: 🎸 DEMANDE BL FONCTIONNEL
</commit_message>
<xml_diff>
--- a/BL/fournisseurs.xlsx
+++ b/BL/fournisseurs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZBAIRI\Desktop\DEV\envoyer_mail_facture\BL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9209AD84-A4DD-4E87-AAAA-97293ED9B7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C358B4-B6C9-44DE-8F02-F51A589AB6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
   <si>
     <t>FOURNISSEUR</t>
   </si>
@@ -265,24 +265,85 @@
   </si>
   <si>
     <t>zmo.salamarket@gmail.com</t>
+  </si>
+  <si>
+    <t>marie-laure.aladenise@puigrenier.fr</t>
+  </si>
+  <si>
+    <t>PUIGRENIER</t>
+  </si>
+  <si>
+    <t>d.girardy@ieupartner.com</t>
+  </si>
+  <si>
+    <t>IFRI</t>
+  </si>
+  <si>
+    <t>service-client13@salamarket.fr</t>
+  </si>
+  <si>
+    <t>K2A MARSEILLE</t>
+  </si>
+  <si>
+    <t>sales@iniciatrade.com</t>
+  </si>
+  <si>
+    <t>INICIA TRADE</t>
+  </si>
+  <si>
+    <t>lucie.kedimi@yfrais.fr</t>
+  </si>
+  <si>
+    <t>camille.baroux@bbmfrance.com</t>
+  </si>
+  <si>
+    <t>BBM</t>
+  </si>
+  <si>
+    <t>TENDRIADE</t>
+  </si>
+  <si>
+    <t>compta.client@tendriade.fr</t>
+  </si>
+  <si>
+    <t>globalfoodcompagny@gmail.com</t>
+  </si>
+  <si>
+    <t>GLOBAL FOOD COMPAGNY</t>
+  </si>
+  <si>
+    <t>info@molinospadoni.it</t>
+  </si>
+  <si>
+    <t>MOLINO SPADONI</t>
+  </si>
+  <si>
+    <t>commande@salamarket.fr</t>
+  </si>
+  <si>
+    <t>SALAMARKET DHM34</t>
+  </si>
+  <si>
+    <t>comptae3f@eurosourcing.fr</t>
+  </si>
+  <si>
+    <t>EUROSOURCING</t>
+  </si>
+  <si>
+    <t>PRO A PRO</t>
+  </si>
+  <si>
+    <t>papfr-montaubansav@proapro.fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,9 +393,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -342,12 +402,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -637,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +722,7 @@
       <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -677,7 +738,7 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -693,7 +754,7 @@
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -701,7 +762,7 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -717,7 +778,7 @@
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -789,7 +850,7 @@
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -853,7 +914,7 @@
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -877,7 +938,7 @@
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -909,7 +970,7 @@
       <c r="A33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -965,15 +1026,15 @@
       <c r="A40" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>13</v>
+      <c r="B40" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -983,6 +1044,94 @@
       </c>
       <c r="B42" s="1" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -992,7 +1141,10 @@
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{5E08EF60-7136-4AE0-9819-B7723291DAC2}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{2385EC7A-0B04-4BDE-8FBD-184FB0ED21AD}"/>
+    <hyperlink ref="B49" r:id="rId3" xr:uid="{8630459F-FE07-49F5-82A8-2FDF0F02CA44}"/>
+    <hyperlink ref="B53" r:id="rId4" xr:uid="{C7EC3C59-48D7-4217-BBE7-E0F637AEA76A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>